<commit_message>
Implemented 3 sessions instead of 2 and updated the excel file
</commit_message>
<xml_diff>
--- a/RATtrials.xlsx
+++ b/RATtrials.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsayali1/Desktop/RAT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsayali1/Documents/Github/RATgame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C9878B-5F3B-6A41-ABB7-AB4AC7BDDABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ED74DD-73AE-4D4A-9098-01237B92C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="21500" windowHeight="14980" xr2:uid="{DD858641-4BA8-C24A-A4B0-B322AA328019}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="345">
   <si>
     <t>TrialType</t>
   </si>
@@ -804,9 +804,6 @@
     <t>ship</t>
   </si>
   <si>
-    <t>battles</t>
-  </si>
-  <si>
     <t>hold</t>
   </si>
   <si>
@@ -1066,6 +1063,12 @@
   </si>
   <si>
     <t>TestDay</t>
+  </si>
+  <si>
+    <t>ParticipantsSolving</t>
+  </si>
+  <si>
+    <t>battle</t>
   </si>
 </sst>
 </file>
@@ -1417,15 +1420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D9DEF1-74EA-B14D-BF06-3599EA10F0E6}">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1442,13 +1445,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G1" t="s">
+        <v>342</v>
+      </c>
+      <c r="H1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1470,8 +1476,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1493,1388 +1502,1571 @@
       <c r="G3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>30</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D14" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F14" t="s">
         <v>42</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17">
+      <c r="H17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="G19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23">
+      <c r="H23">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="G25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" t="s">
-        <v>113</v>
-      </c>
-      <c r="E29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G29">
+      <c r="H29">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="E31" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="F31" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="G31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>275</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>276</v>
       </c>
       <c r="E32" t="s">
-        <v>126</v>
+        <v>277</v>
       </c>
       <c r="F32" t="s">
-        <v>127</v>
+        <v>278</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>279</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>280</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>281</v>
       </c>
       <c r="F33" t="s">
-        <v>131</v>
+        <v>282</v>
       </c>
       <c r="G33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="F34" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>183</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>184</v>
+      </c>
+      <c r="F35" t="s">
+        <v>185</v>
+      </c>
+      <c r="G35">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35">
+      <c r="H35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E36" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" t="s">
+        <v>189</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
         <v>34</v>
       </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36">
-        <v>35</v>
-      </c>
-      <c r="C36" t="s">
-        <v>140</v>
-      </c>
-      <c r="D36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" t="s">
-        <v>142</v>
-      </c>
-      <c r="F36" t="s">
-        <v>143</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="D37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" t="s">
+        <v>192</v>
+      </c>
+      <c r="F37" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" t="s">
         <v>87</v>
       </c>
-      <c r="E37" t="s">
-        <v>145</v>
-      </c>
-      <c r="F37" t="s">
-        <v>146</v>
-      </c>
-      <c r="G37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38">
-        <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" t="s">
-        <v>149</v>
-      </c>
       <c r="F38" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
       <c r="B39">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="F39" t="s">
-        <v>154</v>
+        <v>92</v>
       </c>
       <c r="G39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>283</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>284</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="F40" t="s">
-        <v>157</v>
+        <v>285</v>
       </c>
       <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>286</v>
+      </c>
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="s">
+        <v>287</v>
+      </c>
+      <c r="F41" t="s">
+        <v>288</v>
+      </c>
+      <c r="G41">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" t="s">
-        <v>160</v>
-      </c>
-      <c r="F41" t="s">
-        <v>161</v>
-      </c>
-      <c r="G41">
+      <c r="H41">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>51</v>
+      </c>
+      <c r="C42" t="s">
+        <v>194</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" t="s">
-        <v>83</v>
-      </c>
-      <c r="F42" t="s">
-        <v>163</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="D43" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="E43" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="F43" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="G43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
       <c r="B45">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>96</v>
       </c>
       <c r="D45" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="F45" t="s">
-        <v>173</v>
+        <v>99</v>
       </c>
       <c r="G45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" t="s">
+        <v>203</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>204</v>
+      </c>
+      <c r="D47" t="s">
+        <v>205</v>
+      </c>
+      <c r="E47" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" t="s">
+        <v>206</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" t="s">
+        <v>208</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" t="s">
+        <v>210</v>
+      </c>
+      <c r="E49" t="s">
+        <v>211</v>
+      </c>
+      <c r="F49" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>289</v>
+      </c>
+      <c r="D50" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E46" t="s">
-        <v>176</v>
-      </c>
-      <c r="F46" t="s">
-        <v>177</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47">
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" t="s">
-        <v>179</v>
-      </c>
-      <c r="E47" t="s">
-        <v>39</v>
-      </c>
-      <c r="F47" t="s">
-        <v>180</v>
-      </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E48" t="s">
-        <v>181</v>
-      </c>
-      <c r="F48" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>183</v>
-      </c>
-      <c r="D49" t="s">
-        <v>108</v>
-      </c>
-      <c r="E49" t="s">
-        <v>184</v>
-      </c>
-      <c r="F49" t="s">
-        <v>185</v>
-      </c>
-      <c r="G49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50">
-        <v>49</v>
-      </c>
-      <c r="C50" t="s">
-        <v>186</v>
-      </c>
-      <c r="D50" t="s">
-        <v>187</v>
-      </c>
       <c r="E50" t="s">
-        <v>188</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
-        <v>189</v>
+        <v>290</v>
       </c>
       <c r="G50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>190</v>
+        <v>291</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E51" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="F51" t="s">
-        <v>193</v>
+        <v>292</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="D52" t="s">
-        <v>116</v>
+        <v>214</v>
       </c>
       <c r="E52" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="F52" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" t="s">
+        <v>217</v>
+      </c>
+      <c r="E53" t="s">
+        <v>218</v>
+      </c>
+      <c r="F53" t="s">
+        <v>219</v>
+      </c>
+      <c r="G53">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>197</v>
-      </c>
-      <c r="D53" t="s">
-        <v>198</v>
-      </c>
-      <c r="E53" t="s">
-        <v>199</v>
-      </c>
-      <c r="F53" t="s">
-        <v>200</v>
-      </c>
-      <c r="G53">
+      <c r="H53">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" t="s">
+        <v>102</v>
+      </c>
+      <c r="F54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G54">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54">
-        <v>53</v>
-      </c>
-      <c r="C54" t="s">
-        <v>201</v>
-      </c>
-      <c r="D54" t="s">
-        <v>202</v>
-      </c>
-      <c r="E54" t="s">
-        <v>90</v>
-      </c>
-      <c r="F54" t="s">
-        <v>203</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
       <c r="B55">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="D55" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
       <c r="E55" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="F55" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="G55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
       <c r="B56">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>294</v>
       </c>
       <c r="E56" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="F56" t="s">
-        <v>208</v>
+        <v>295</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
       <c r="B57">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>209</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
-        <v>210</v>
+        <v>117</v>
       </c>
       <c r="E57" t="s">
-        <v>211</v>
+        <v>296</v>
       </c>
       <c r="F57" t="s">
-        <v>212</v>
+        <v>297</v>
       </c>
       <c r="G57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
       <c r="B58">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D58" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E58" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="F58" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F59" t="s">
+        <v>224</v>
+      </c>
+      <c r="G59">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59">
-        <v>58</v>
-      </c>
-      <c r="C59" t="s">
-        <v>83</v>
-      </c>
-      <c r="D59" t="s">
-        <v>217</v>
-      </c>
-      <c r="E59" t="s">
-        <v>218</v>
-      </c>
-      <c r="F59" t="s">
-        <v>219</v>
-      </c>
-      <c r="G59">
+      <c r="H59">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" t="s">
+        <v>225</v>
+      </c>
+      <c r="E60" t="s">
+        <v>226</v>
+      </c>
+      <c r="F60" t="s">
+        <v>227</v>
+      </c>
+      <c r="G60">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60">
-        <v>59</v>
-      </c>
-      <c r="C60" t="s">
-        <v>220</v>
-      </c>
-      <c r="D60" t="s">
-        <v>221</v>
-      </c>
-      <c r="E60" t="s">
-        <v>222</v>
-      </c>
-      <c r="F60" t="s">
-        <v>211</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
       <c r="B61">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>65</v>
+        <v>228</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>229</v>
       </c>
       <c r="E61" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="F61" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="G61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
       <c r="B62">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="C62" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D62" t="s">
-        <v>225</v>
+        <v>109</v>
       </c>
       <c r="E62" t="s">
-        <v>226</v>
+        <v>110</v>
       </c>
       <c r="F62" t="s">
-        <v>227</v>
+        <v>111</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
       <c r="B63">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C63" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="D63" t="s">
-        <v>229</v>
+        <v>113</v>
       </c>
       <c r="E63" t="s">
-        <v>230</v>
+        <v>114</v>
       </c>
       <c r="F63" t="s">
-        <v>231</v>
+        <v>115</v>
       </c>
       <c r="G63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -2894,10 +3086,13 @@
         <v>234</v>
       </c>
       <c r="G64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H64">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -2917,608 +3112,689 @@
         <v>238</v>
       </c>
       <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>83</v>
+      </c>
+      <c r="C66" t="s">
+        <v>225</v>
+      </c>
+      <c r="D66" t="s">
+        <v>298</v>
+      </c>
+      <c r="E66" t="s">
+        <v>299</v>
+      </c>
+      <c r="F66" t="s">
+        <v>300</v>
+      </c>
+      <c r="G66">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66">
-        <v>65</v>
-      </c>
-      <c r="C66" t="s">
-        <v>239</v>
-      </c>
-      <c r="D66" t="s">
-        <v>240</v>
-      </c>
-      <c r="E66" t="s">
-        <v>241</v>
-      </c>
-      <c r="F66" t="s">
-        <v>242</v>
-      </c>
-      <c r="G66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="B67">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
-        <v>243</v>
+        <v>301</v>
       </c>
       <c r="D67" t="s">
-        <v>244</v>
+        <v>105</v>
       </c>
       <c r="E67" t="s">
-        <v>202</v>
+        <v>302</v>
       </c>
       <c r="F67" t="s">
-        <v>245</v>
+        <v>303</v>
       </c>
       <c r="G67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
       <c r="B68">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>246</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
-        <v>247</v>
+        <v>117</v>
       </c>
       <c r="E68" t="s">
-        <v>248</v>
+        <v>118</v>
       </c>
       <c r="F68" t="s">
-        <v>214</v>
+        <v>119</v>
       </c>
       <c r="G68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
       <c r="B69">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s">
-        <v>249</v>
+        <v>120</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
+        <v>121</v>
       </c>
       <c r="E69" t="s">
-        <v>251</v>
+        <v>122</v>
       </c>
       <c r="F69" t="s">
-        <v>252</v>
+        <v>123</v>
       </c>
       <c r="G69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
       <c r="B70">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="D70" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
       <c r="E70" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="F70" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>86</v>
+      </c>
+      <c r="C71" t="s">
+        <v>308</v>
+      </c>
+      <c r="D71" t="s">
+        <v>309</v>
+      </c>
+      <c r="E71" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" t="s">
+        <v>310</v>
+      </c>
+      <c r="G71">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>257</v>
-      </c>
-      <c r="D71" t="s">
-        <v>258</v>
-      </c>
-      <c r="E71" t="s">
-        <v>259</v>
-      </c>
-      <c r="F71" t="s">
-        <v>260</v>
-      </c>
-      <c r="G71">
+      <c r="H71">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>65</v>
+      </c>
+      <c r="C72" t="s">
+        <v>239</v>
+      </c>
+      <c r="D72" t="s">
+        <v>240</v>
+      </c>
+      <c r="E72" t="s">
+        <v>241</v>
+      </c>
+      <c r="F72" t="s">
+        <v>242</v>
+      </c>
+      <c r="G72">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72">
-        <v>71</v>
-      </c>
-      <c r="C72" t="s">
-        <v>261</v>
-      </c>
-      <c r="D72" t="s">
-        <v>262</v>
-      </c>
-      <c r="E72" t="s">
-        <v>263</v>
-      </c>
-      <c r="F72" t="s">
-        <v>264</v>
-      </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
       <c r="B73">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="D73" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="E73" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="F73" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="G73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C74" t="s">
-        <v>268</v>
+        <v>311</v>
       </c>
       <c r="D74" t="s">
-        <v>269</v>
+        <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="F74" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="G74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>60</v>
       </c>
       <c r="D75" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="E75" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="F75" t="s">
-        <v>275</v>
+        <v>316</v>
       </c>
       <c r="G75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C76" t="s">
-        <v>276</v>
+        <v>246</v>
       </c>
       <c r="D76" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="E76" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="F76" t="s">
-        <v>279</v>
+        <v>214</v>
       </c>
       <c r="G76">
+        <v>3</v>
+      </c>
+      <c r="H76">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>68</v>
+      </c>
+      <c r="C77" t="s">
+        <v>249</v>
+      </c>
+      <c r="D77" t="s">
+        <v>250</v>
+      </c>
+      <c r="E77" t="s">
+        <v>251</v>
+      </c>
+      <c r="F77" t="s">
+        <v>252</v>
+      </c>
+      <c r="G77">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77">
-        <v>76</v>
-      </c>
-      <c r="C77" t="s">
-        <v>280</v>
-      </c>
-      <c r="D77" t="s">
-        <v>281</v>
-      </c>
-      <c r="E77" t="s">
-        <v>282</v>
-      </c>
-      <c r="F77" t="s">
-        <v>283</v>
-      </c>
-      <c r="G77">
+      <c r="H77">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>31</v>
+      </c>
+      <c r="C78" t="s">
+        <v>124</v>
+      </c>
+      <c r="D78" t="s">
+        <v>125</v>
+      </c>
+      <c r="E78" t="s">
+        <v>126</v>
+      </c>
+      <c r="F78" t="s">
+        <v>127</v>
+      </c>
+      <c r="G78">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78">
-        <v>77</v>
-      </c>
-      <c r="C78" t="s">
-        <v>284</v>
-      </c>
-      <c r="D78" t="s">
-        <v>285</v>
-      </c>
-      <c r="E78" t="s">
-        <v>105</v>
-      </c>
-      <c r="F78" t="s">
-        <v>286</v>
-      </c>
-      <c r="G78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
       <c r="B79">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="C79" t="s">
-        <v>287</v>
+        <v>128</v>
       </c>
       <c r="D79" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
       <c r="E79" t="s">
-        <v>288</v>
+        <v>130</v>
       </c>
       <c r="F79" t="s">
-        <v>289</v>
+        <v>131</v>
       </c>
       <c r="G79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H79">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
       <c r="B80">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="D80" t="s">
-        <v>45</v>
+        <v>254</v>
       </c>
       <c r="E80" t="s">
-        <v>116</v>
+        <v>255</v>
       </c>
       <c r="F80" t="s">
-        <v>291</v>
+        <v>344</v>
       </c>
       <c r="G80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
       <c r="B81">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C81" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="D81" t="s">
-        <v>187</v>
+        <v>257</v>
       </c>
       <c r="E81" t="s">
-        <v>209</v>
+        <v>258</v>
       </c>
       <c r="F81" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
       <c r="G81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
       <c r="B82">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C82" t="s">
-        <v>294</v>
+        <v>260</v>
       </c>
       <c r="D82" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
       <c r="E82" t="s">
+        <v>262</v>
+      </c>
+      <c r="F82" t="s">
+        <v>263</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+      <c r="H82">
         <v>9</v>
       </c>
-      <c r="F82" t="s">
-        <v>296</v>
-      </c>
-      <c r="G82">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>72</v>
+      </c>
+      <c r="C83" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" t="s">
+        <v>264</v>
+      </c>
+      <c r="E83" t="s">
+        <v>265</v>
+      </c>
+      <c r="F83" t="s">
+        <v>266</v>
+      </c>
+      <c r="G83">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83">
-        <v>82</v>
-      </c>
-      <c r="C83" t="s">
-        <v>144</v>
-      </c>
-      <c r="D83" t="s">
-        <v>117</v>
-      </c>
-      <c r="E83" t="s">
-        <v>297</v>
-      </c>
-      <c r="F83" t="s">
-        <v>298</v>
-      </c>
-      <c r="G83">
+      <c r="H83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>89</v>
+      </c>
+      <c r="C84" t="s">
+        <v>317</v>
+      </c>
+      <c r="D84" t="s">
+        <v>318</v>
+      </c>
+      <c r="E84" t="s">
+        <v>319</v>
+      </c>
+      <c r="F84" t="s">
+        <v>320</v>
+      </c>
+      <c r="G84">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84">
-        <v>83</v>
-      </c>
-      <c r="C84" t="s">
-        <v>225</v>
-      </c>
-      <c r="D84" t="s">
-        <v>299</v>
-      </c>
-      <c r="E84" t="s">
-        <v>300</v>
-      </c>
-      <c r="F84" t="s">
-        <v>301</v>
-      </c>
-      <c r="G84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
       <c r="B85">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C85" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="D85" t="s">
-        <v>105</v>
+        <v>322</v>
       </c>
       <c r="E85" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="F85" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="G85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H85">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
       <c r="B86">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C86" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="D86" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="E86" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="F86" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="G86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
       <c r="B87">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C87" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="D87" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="E87" t="s">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="F87" t="s">
-        <v>311</v>
+        <v>274</v>
       </c>
       <c r="G87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
       <c r="B88">
+        <v>33</v>
+      </c>
+      <c r="C88" t="s">
+        <v>132</v>
+      </c>
+      <c r="D88" t="s">
+        <v>133</v>
+      </c>
+      <c r="E88" t="s">
+        <v>134</v>
+      </c>
+      <c r="F88" t="s">
+        <v>135</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="H88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>34</v>
+      </c>
+      <c r="C89" t="s">
+        <v>136</v>
+      </c>
+      <c r="D89" t="s">
+        <v>137</v>
+      </c>
+      <c r="E89" t="s">
+        <v>138</v>
+      </c>
+      <c r="F89" t="s">
+        <v>139</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>35</v>
+      </c>
+      <c r="C90" t="s">
+        <v>140</v>
+      </c>
+      <c r="D90" t="s">
+        <v>141</v>
+      </c>
+      <c r="E90" t="s">
+        <v>142</v>
+      </c>
+      <c r="F90" t="s">
+        <v>143</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>36</v>
+      </c>
+      <c r="C91" t="s">
+        <v>144</v>
+      </c>
+      <c r="D91" t="s">
         <v>87</v>
       </c>
-      <c r="C88" t="s">
-        <v>312</v>
-      </c>
-      <c r="D88" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" t="s">
-        <v>313</v>
-      </c>
-      <c r="F88" t="s">
-        <v>314</v>
-      </c>
-      <c r="G88">
+      <c r="E91" t="s">
+        <v>145</v>
+      </c>
+      <c r="F91" t="s">
+        <v>146</v>
+      </c>
+      <c r="G91">
+        <v>3</v>
+      </c>
+      <c r="H91">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89">
-        <v>88</v>
-      </c>
-      <c r="C89" t="s">
-        <v>60</v>
-      </c>
-      <c r="D89" t="s">
-        <v>315</v>
-      </c>
-      <c r="E89" t="s">
-        <v>316</v>
-      </c>
-      <c r="F89" t="s">
-        <v>317</v>
-      </c>
-      <c r="G89">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90">
-        <v>89</v>
-      </c>
-      <c r="C90" t="s">
-        <v>318</v>
-      </c>
-      <c r="D90" t="s">
-        <v>319</v>
-      </c>
-      <c r="E90" t="s">
-        <v>320</v>
-      </c>
-      <c r="F90" t="s">
-        <v>321</v>
-      </c>
-      <c r="G90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91">
-        <v>90</v>
-      </c>
-      <c r="C91" t="s">
-        <v>322</v>
-      </c>
-      <c r="D91" t="s">
-        <v>323</v>
-      </c>
-      <c r="E91" t="s">
-        <v>324</v>
-      </c>
-      <c r="F91" t="s">
-        <v>325</v>
-      </c>
-      <c r="G91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -3526,22 +3802,25 @@
         <v>101</v>
       </c>
       <c r="C92" t="s">
+        <v>326</v>
+      </c>
+      <c r="D92" t="s">
         <v>327</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>328</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>329</v>
-      </c>
-      <c r="F92" t="s">
-        <v>330</v>
       </c>
       <c r="G92">
         <v>999</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -3549,22 +3828,25 @@
         <v>102</v>
       </c>
       <c r="C93" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D93" t="s">
+        <v>330</v>
+      </c>
+      <c r="E93" t="s">
         <v>331</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>332</v>
-      </c>
-      <c r="F93" t="s">
-        <v>333</v>
       </c>
       <c r="G93">
         <v>999</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -3575,19 +3857,22 @@
         <v>105</v>
       </c>
       <c r="D94" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E94" t="s">
         <v>67</v>
       </c>
       <c r="F94" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G94">
         <v>999</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -3595,22 +3880,25 @@
         <v>104</v>
       </c>
       <c r="C95" t="s">
+        <v>335</v>
+      </c>
+      <c r="D95" t="s">
         <v>336</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>337</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>338</v>
-      </c>
-      <c r="F95" t="s">
-        <v>339</v>
       </c>
       <c r="G95">
         <v>999</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -3618,22 +3906,29 @@
         <v>105</v>
       </c>
       <c r="C96" t="s">
+        <v>339</v>
+      </c>
+      <c r="D96" t="s">
         <v>340</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>341</v>
       </c>
-      <c r="E96" t="s">
-        <v>342</v>
-      </c>
       <c r="F96" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G96">
         <v>999</v>
       </c>
+      <c r="H96">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H99">
+    <sortCondition descending="1" ref="A2:A99"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doubled response deadline and changed RAT words per session
</commit_message>
<xml_diff>
--- a/RATtrials.xlsx
+++ b/RATtrials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsayali1/Documents/Github/RATgame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ED74DD-73AE-4D4A-9098-01237B92C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A869962-F09C-174E-8D83-0B545F75AC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="21500" windowHeight="14980" xr2:uid="{DD858641-4BA8-C24A-A4B0-B322AA328019}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="21820" windowHeight="15840" xr2:uid="{DD858641-4BA8-C24A-A4B0-B322AA328019}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="346">
   <si>
     <t>TrialType</t>
   </si>
@@ -777,9 +777,6 @@
     <t>grass</t>
   </si>
   <si>
-    <t>kind</t>
-  </si>
-  <si>
     <t>meat</t>
   </si>
   <si>
@@ -1065,10 +1062,16 @@
     <t>TestDay</t>
   </si>
   <si>
-    <t>ParticipantsSolving</t>
-  </si>
-  <si>
     <t>battle</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>ParticipantsSolving15</t>
+  </si>
+  <si>
+    <t>ParticipantsSolving30</t>
   </si>
 </sst>
 </file>
@@ -1420,15 +1423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D9DEF1-74EA-B14D-BF06-3599EA10F0E6}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1445,42 +1448,48 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+      <c r="I1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="I2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1500,2275 +1509,2539 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="I5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="I6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>66</v>
+      </c>
+      <c r="I7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>163</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="I8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="I9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="I10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>285</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>286</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>287</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="I11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>295</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>296</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="I12">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="F13" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="I13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>33</v>
+      </c>
+      <c r="I15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>30</v>
+      </c>
+      <c r="I16">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
         <v>46</v>
       </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>163</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>42</v>
-      </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I17">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>217</v>
       </c>
       <c r="E18" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>26</v>
+      </c>
+      <c r="I18">
         <v>49</v>
       </c>
-      <c r="F18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>188</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>189</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="I19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="I20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>290</v>
       </c>
       <c r="D21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F21" t="s">
+        <v>291</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>28</v>
+      </c>
+      <c r="I21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" t="s">
+        <v>234</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>18</v>
+      </c>
+      <c r="I22">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
         <v>60</v>
       </c>
-      <c r="E21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>167</v>
-      </c>
-      <c r="D22" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>169</v>
-      </c>
-      <c r="G22">
-        <v>3</v>
-      </c>
-      <c r="H22">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>44</v>
-      </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="I23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>225</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>226</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>227</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="I24">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>310</v>
       </c>
       <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>311</v>
+      </c>
+      <c r="F25" t="s">
+        <v>312</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>14</v>
+      </c>
+      <c r="I25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25">
-        <v>3</v>
-      </c>
-      <c r="H25">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>17</v>
-      </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>249</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>251</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="I26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>270</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>271</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>272</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
+        <v>273</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="I28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>307</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>308</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>84</v>
+        <v>309</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="I29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" t="s">
+        <v>143</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
         <v>45</v>
       </c>
-      <c r="C30" t="s">
-        <v>174</v>
-      </c>
-      <c r="D30" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30">
+      <c r="D31" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" t="s">
+        <v>264</v>
+      </c>
+      <c r="F31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>9</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32">
         <v>2</v>
       </c>
-      <c r="H30">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
-        <v>178</v>
-      </c>
-      <c r="D31" t="s">
-        <v>179</v>
-      </c>
-      <c r="E31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" t="s">
-        <v>180</v>
-      </c>
-      <c r="G31">
-        <v>3</v>
-      </c>
-      <c r="H31">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32">
-        <v>75</v>
-      </c>
-      <c r="C32" t="s">
-        <v>275</v>
-      </c>
-      <c r="D32" t="s">
-        <v>276</v>
-      </c>
-      <c r="E32" t="s">
-        <v>277</v>
-      </c>
-      <c r="F32" t="s">
-        <v>278</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
       <c r="H32">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="I32">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>279</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>280</v>
+        <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>281</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>282</v>
+        <v>26</v>
       </c>
       <c r="G33">
         <v>2</v>
       </c>
       <c r="H33">
+        <v>68</v>
+      </c>
+      <c r="I33">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>53</v>
+      </c>
+      <c r="I34">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34">
-        <v>47</v>
-      </c>
-      <c r="C34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" t="s">
-        <v>171</v>
-      </c>
-      <c r="E34" t="s">
-        <v>181</v>
-      </c>
-      <c r="F34" t="s">
-        <v>182</v>
-      </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-      <c r="H34">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35">
-        <v>48</v>
-      </c>
-      <c r="C35" t="s">
-        <v>183</v>
-      </c>
-      <c r="D35" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" t="s">
-        <v>184</v>
-      </c>
-      <c r="F35" t="s">
-        <v>185</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E36" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F36" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="G36">
         <v>2</v>
       </c>
       <c r="H36">
+        <v>41</v>
+      </c>
+      <c r="I36">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>46</v>
+      </c>
+      <c r="I37">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>63</v>
+      </c>
+      <c r="I38">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37">
-        <v>50</v>
-      </c>
-      <c r="C37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" t="s">
-        <v>191</v>
-      </c>
-      <c r="E37" t="s">
-        <v>192</v>
-      </c>
-      <c r="F37" t="s">
-        <v>193</v>
-      </c>
-      <c r="G37">
-        <v>3</v>
-      </c>
-      <c r="H37">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38">
-        <v>21</v>
-      </c>
-      <c r="C38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" t="s">
-        <v>88</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39">
-        <v>22</v>
-      </c>
-      <c r="C39" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" t="s">
-        <v>92</v>
       </c>
       <c r="G39">
         <v>2</v>
       </c>
       <c r="H39">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="I39">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>278</v>
+      </c>
+      <c r="D40" t="s">
+        <v>279</v>
+      </c>
+      <c r="E40" t="s">
+        <v>280</v>
+      </c>
+      <c r="F40" t="s">
+        <v>281</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>41</v>
+      </c>
+      <c r="I40">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" t="s">
         <v>77</v>
       </c>
-      <c r="C40" t="s">
-        <v>283</v>
-      </c>
-      <c r="D40" t="s">
-        <v>284</v>
-      </c>
-      <c r="E40" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" t="s">
-        <v>285</v>
-      </c>
-      <c r="G40">
-        <v>3</v>
-      </c>
-      <c r="H40">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41">
+      <c r="F41" t="s">
         <v>78</v>
       </c>
-      <c r="C41" t="s">
-        <v>286</v>
-      </c>
-      <c r="D41" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" t="s">
-        <v>287</v>
-      </c>
-      <c r="F41" t="s">
-        <v>288</v>
-      </c>
       <c r="G41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H41">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="I41">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D42" t="s">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="E42" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="F42" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="G42">
         <v>2</v>
       </c>
       <c r="H42">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="I42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>197</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>198</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="F43" t="s">
-        <v>200</v>
+        <v>107</v>
       </c>
       <c r="G43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H43">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="I43">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H44">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="I44">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
       <c r="B45">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>209</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>210</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>211</v>
       </c>
       <c r="F45" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="G45">
         <v>2</v>
       </c>
       <c r="H45">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="I45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D46" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E46" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F46" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H46">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>171</v>
+      </c>
+      <c r="E47" t="s">
+        <v>181</v>
+      </c>
+      <c r="F47" t="s">
+        <v>182</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>39</v>
+      </c>
+      <c r="I47">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" t="s">
         <v>54</v>
-      </c>
-      <c r="C47" t="s">
-        <v>204</v>
-      </c>
-      <c r="D47" t="s">
-        <v>205</v>
-      </c>
-      <c r="E47" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" t="s">
-        <v>206</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
-      </c>
-      <c r="H47">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48">
-        <v>55</v>
-      </c>
-      <c r="C48" t="s">
-        <v>207</v>
-      </c>
-      <c r="D48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F48" t="s">
-        <v>208</v>
       </c>
       <c r="G48">
         <v>2</v>
       </c>
       <c r="H48">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="I48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
       <c r="B49">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>209</v>
+        <v>316</v>
       </c>
       <c r="D49" t="s">
-        <v>210</v>
+        <v>317</v>
       </c>
       <c r="E49" t="s">
-        <v>211</v>
+        <v>318</v>
       </c>
       <c r="F49" t="s">
-        <v>212</v>
+        <v>319</v>
       </c>
       <c r="G49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H49">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="I49">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>289</v>
+        <v>228</v>
       </c>
       <c r="D50" t="s">
-        <v>45</v>
+        <v>229</v>
       </c>
       <c r="E50" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
       <c r="F50" t="s">
-        <v>290</v>
+        <v>231</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H50">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="I50">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>291</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>187</v>
+        <v>121</v>
       </c>
       <c r="E51" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="F51" t="s">
-        <v>292</v>
+        <v>123</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
       <c r="H51">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="I51">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>213</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>214</v>
+        <v>129</v>
       </c>
       <c r="E52" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
       <c r="F52" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H52">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I52">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>217</v>
+        <v>97</v>
       </c>
       <c r="E53" t="s">
-        <v>218</v>
+        <v>98</v>
       </c>
       <c r="F53" t="s">
-        <v>219</v>
+        <v>99</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H53">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="I53">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="D54" t="s">
-        <v>101</v>
+        <v>240</v>
       </c>
       <c r="E54" t="s">
-        <v>102</v>
+        <v>241</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="G54">
         <v>2</v>
       </c>
       <c r="H54">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I54">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
       <c r="B55">
+        <v>79</v>
+      </c>
+      <c r="C55" t="s">
+        <v>288</v>
+      </c>
+      <c r="D55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" t="s">
+        <v>289</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>28</v>
+      </c>
+      <c r="I55">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>66</v>
+      </c>
+      <c r="C56" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" t="s">
+        <v>244</v>
+      </c>
+      <c r="E56" t="s">
+        <v>202</v>
+      </c>
+      <c r="F56" t="s">
+        <v>245</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56">
+        <v>16</v>
+      </c>
+      <c r="I56">
         <v>26</v>
       </c>
-      <c r="C55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" t="s">
-        <v>105</v>
-      </c>
-      <c r="E55" t="s">
-        <v>106</v>
-      </c>
-      <c r="F55" t="s">
-        <v>107</v>
-      </c>
-      <c r="G55">
-        <v>3</v>
-      </c>
-      <c r="H55">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56">
-        <v>81</v>
-      </c>
-      <c r="C56" t="s">
-        <v>293</v>
-      </c>
-      <c r="D56" t="s">
-        <v>294</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" t="s">
-        <v>295</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
       <c r="B57">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>144</v>
+        <v>246</v>
       </c>
       <c r="D57" t="s">
-        <v>117</v>
+        <v>343</v>
       </c>
       <c r="E57" t="s">
-        <v>296</v>
+        <v>247</v>
       </c>
       <c r="F57" t="s">
-        <v>297</v>
+        <v>214</v>
       </c>
       <c r="G57">
         <v>2</v>
       </c>
       <c r="H57">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="I57">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
       <c r="B58">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="D58" t="s">
-        <v>221</v>
+        <v>116</v>
       </c>
       <c r="E58" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="F58" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="G58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H58">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="I58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
       <c r="B59">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="E59" t="s">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="F59" t="s">
-        <v>224</v>
+        <v>119</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H59">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="I59">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
       <c r="B60">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
       <c r="D60" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="E60" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="F60" t="s">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="G60">
         <v>2</v>
       </c>
       <c r="H60">
+        <v>7</v>
+      </c>
+      <c r="I60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>34</v>
+      </c>
+      <c r="C61" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" t="s">
+        <v>138</v>
+      </c>
+      <c r="F61" t="s">
+        <v>139</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <v>5</v>
+      </c>
+      <c r="I61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>40</v>
+      </c>
+      <c r="C62" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" t="s">
+        <v>160</v>
+      </c>
+      <c r="F62" t="s">
+        <v>161</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <v>66</v>
+      </c>
+      <c r="I62">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="H63">
+        <v>61</v>
+      </c>
+      <c r="I63">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61">
-        <v>62</v>
-      </c>
-      <c r="C61" t="s">
-        <v>228</v>
-      </c>
-      <c r="D61" t="s">
-        <v>229</v>
-      </c>
-      <c r="E61" t="s">
-        <v>230</v>
-      </c>
-      <c r="F61" t="s">
-        <v>231</v>
-      </c>
-      <c r="G61">
-        <v>3</v>
-      </c>
-      <c r="H61">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62">
-        <v>27</v>
-      </c>
-      <c r="C62" t="s">
-        <v>108</v>
-      </c>
-      <c r="D62" t="s">
-        <v>109</v>
-      </c>
-      <c r="E62" t="s">
-        <v>110</v>
-      </c>
-      <c r="F62" t="s">
-        <v>111</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="H62">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63">
-        <v>28</v>
-      </c>
-      <c r="C63" t="s">
-        <v>112</v>
-      </c>
-      <c r="D63" t="s">
-        <v>113</v>
-      </c>
-      <c r="E63" t="s">
-        <v>114</v>
-      </c>
-      <c r="F63" t="s">
-        <v>115</v>
-      </c>
-      <c r="G63">
-        <v>2</v>
-      </c>
-      <c r="H63">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64">
-        <v>63</v>
-      </c>
-      <c r="C64" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" t="s">
-        <v>232</v>
-      </c>
-      <c r="E64" t="s">
-        <v>233</v>
-      </c>
-      <c r="F64" t="s">
-        <v>234</v>
       </c>
       <c r="G64">
         <v>3</v>
       </c>
       <c r="H64">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="I64">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>235</v>
+        <v>81</v>
       </c>
       <c r="D65" t="s">
-        <v>236</v>
+        <v>82</v>
       </c>
       <c r="E65" t="s">
-        <v>237</v>
+        <v>83</v>
       </c>
       <c r="F65" t="s">
-        <v>238</v>
+        <v>84</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H65">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I65">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
       <c r="B66">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>225</v>
+        <v>147</v>
       </c>
       <c r="D66" t="s">
-        <v>298</v>
+        <v>148</v>
       </c>
       <c r="E66" t="s">
-        <v>299</v>
+        <v>149</v>
       </c>
       <c r="F66" t="s">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="G66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="I66">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="B67">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>301</v>
+        <v>59</v>
       </c>
       <c r="D67" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="E67" t="s">
-        <v>302</v>
+        <v>61</v>
       </c>
       <c r="F67" t="s">
-        <v>303</v>
+        <v>62</v>
       </c>
       <c r="G67">
         <v>3</v>
       </c>
       <c r="H67">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="I67">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
       <c r="B68">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="D68" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="E68" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="F68" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>42</v>
+      </c>
+      <c r="I68">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>190</v>
+      </c>
+      <c r="D69" t="s">
+        <v>191</v>
+      </c>
+      <c r="E69" t="s">
+        <v>192</v>
+      </c>
+      <c r="F69" t="s">
+        <v>193</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69">
+        <v>34</v>
+      </c>
+      <c r="I69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
         <v>1</v>
       </c>
-      <c r="H68">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69">
-        <v>30</v>
-      </c>
-      <c r="C69" t="s">
-        <v>120</v>
-      </c>
-      <c r="D69" t="s">
-        <v>121</v>
-      </c>
-      <c r="E69" t="s">
-        <v>122</v>
-      </c>
-      <c r="F69" t="s">
-        <v>123</v>
-      </c>
-      <c r="G69">
-        <v>2</v>
-      </c>
-      <c r="H69">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>5</v>
-      </c>
-      <c r="B70">
-        <v>85</v>
-      </c>
       <c r="C70" t="s">
-        <v>304</v>
+        <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>306</v>
+        <v>9</v>
       </c>
       <c r="F70" t="s">
-        <v>307</v>
+        <v>19</v>
       </c>
       <c r="G70">
         <v>3</v>
       </c>
       <c r="H70">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="I70">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
       <c r="B71">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="D71" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="E71" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="F71" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H71">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="I71">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
       <c r="B72">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>239</v>
+        <v>274</v>
       </c>
       <c r="D72" t="s">
-        <v>240</v>
+        <v>275</v>
       </c>
       <c r="E72" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="F72" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="G72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H72">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I72">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
       <c r="B73">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>244</v>
+        <v>11</v>
       </c>
       <c r="E73" t="s">
-        <v>202</v>
+        <v>67</v>
       </c>
       <c r="F73" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="I73">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
       <c r="B74">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C74" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>304</v>
       </c>
       <c r="E74" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="F74" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H74">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="I74">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="C75" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="D75" t="s">
-        <v>314</v>
+        <v>109</v>
       </c>
       <c r="E75" t="s">
-        <v>315</v>
+        <v>110</v>
       </c>
       <c r="F75" t="s">
-        <v>316</v>
+        <v>111</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="I75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="D76" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="E76" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="F76" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G76">
         <v>3</v>
       </c>
       <c r="H76">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="I76">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
       <c r="B77">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C77" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="D77" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="E77" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="F77" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H77">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="I77">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
       <c r="B78">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C78" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="D78" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E78" t="s">
-        <v>126</v>
+        <v>184</v>
       </c>
       <c r="F78" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H78">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I78">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
       <c r="B79">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C79" t="s">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="D79" t="s">
-        <v>129</v>
+        <v>321</v>
       </c>
       <c r="E79" t="s">
-        <v>130</v>
+        <v>322</v>
       </c>
       <c r="F79" t="s">
-        <v>131</v>
+        <v>323</v>
       </c>
       <c r="G79">
         <v>3</v>
       </c>
       <c r="H79">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="I79">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
       <c r="B80">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="D80" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="E80" t="s">
+        <v>298</v>
+      </c>
+      <c r="F80" t="s">
+        <v>299</v>
+      </c>
+      <c r="G80">
+        <v>3</v>
+      </c>
+      <c r="H80">
+        <v>18</v>
+      </c>
+      <c r="I80">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>81</v>
+      </c>
+      <c r="C81" t="s">
+        <v>292</v>
+      </c>
+      <c r="D81" t="s">
+        <v>293</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>294</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="H81">
+        <v>25</v>
+      </c>
+      <c r="I81">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>70</v>
+      </c>
+      <c r="C82" t="s">
         <v>255</v>
       </c>
-      <c r="F80" t="s">
-        <v>344</v>
-      </c>
-      <c r="G80">
-        <v>1</v>
-      </c>
-      <c r="H80">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81">
-        <v>70</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="D82" t="s">
         <v>256</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E82" t="s">
         <v>257</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F82" t="s">
         <v>258</v>
-      </c>
-      <c r="F81" t="s">
-        <v>259</v>
-      </c>
-      <c r="G81">
-        <v>2</v>
-      </c>
-      <c r="H81">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82">
-        <v>71</v>
-      </c>
-      <c r="C82" t="s">
-        <v>260</v>
-      </c>
-      <c r="D82" t="s">
-        <v>261</v>
-      </c>
-      <c r="E82" t="s">
-        <v>262</v>
-      </c>
-      <c r="F82" t="s">
-        <v>263</v>
       </c>
       <c r="G82">
         <v>3</v>
       </c>
       <c r="H82">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I82">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
       <c r="B83">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C83" t="s">
-        <v>45</v>
+        <v>201</v>
       </c>
       <c r="D83" t="s">
-        <v>264</v>
+        <v>202</v>
       </c>
       <c r="E83" t="s">
-        <v>265</v>
+        <v>90</v>
       </c>
       <c r="F83" t="s">
-        <v>266</v>
+        <v>203</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H83">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="I83">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
       <c r="B84">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="C84" t="s">
-        <v>317</v>
+        <v>213</v>
       </c>
       <c r="D84" t="s">
-        <v>318</v>
+        <v>214</v>
       </c>
       <c r="E84" t="s">
-        <v>319</v>
+        <v>215</v>
       </c>
       <c r="F84" t="s">
-        <v>320</v>
+        <v>216</v>
       </c>
       <c r="G84">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H84">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="I84">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
       <c r="B85">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>321</v>
+        <v>235</v>
       </c>
       <c r="D85" t="s">
-        <v>322</v>
+        <v>236</v>
       </c>
       <c r="E85" t="s">
-        <v>323</v>
+        <v>237</v>
       </c>
       <c r="F85" t="s">
-        <v>324</v>
+        <v>238</v>
       </c>
       <c r="G85">
         <v>3</v>
       </c>
       <c r="H85">
+        <v>18</v>
+      </c>
+      <c r="I85">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>88</v>
+      </c>
+      <c r="C86" t="s">
+        <v>60</v>
+      </c>
+      <c r="D86" t="s">
+        <v>313</v>
+      </c>
+      <c r="E86" t="s">
+        <v>314</v>
+      </c>
+      <c r="F86" t="s">
+        <v>315</v>
+      </c>
+      <c r="G86">
+        <v>3</v>
+      </c>
+      <c r="H86">
+        <v>14</v>
+      </c>
+      <c r="I86">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>71</v>
+      </c>
+      <c r="C87" t="s">
+        <v>259</v>
+      </c>
+      <c r="D87" t="s">
+        <v>260</v>
+      </c>
+      <c r="E87" t="s">
+        <v>261</v>
+      </c>
+      <c r="F87" t="s">
+        <v>262</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86">
-        <v>73</v>
-      </c>
-      <c r="C86" t="s">
-        <v>267</v>
-      </c>
-      <c r="D86" t="s">
-        <v>268</v>
-      </c>
-      <c r="E86" t="s">
-        <v>269</v>
-      </c>
-      <c r="F86" t="s">
-        <v>270</v>
-      </c>
-      <c r="G86">
-        <v>1</v>
-      </c>
-      <c r="H86">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87">
-        <v>74</v>
-      </c>
-      <c r="C87" t="s">
-        <v>271</v>
-      </c>
-      <c r="D87" t="s">
-        <v>272</v>
-      </c>
-      <c r="E87" t="s">
-        <v>273</v>
-      </c>
-      <c r="F87" t="s">
-        <v>274</v>
-      </c>
-      <c r="G87">
-        <v>2</v>
-      </c>
-      <c r="H87">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
       <c r="B88">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>132</v>
+        <v>300</v>
       </c>
       <c r="D88" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="E88" t="s">
-        <v>134</v>
+        <v>301</v>
       </c>
       <c r="F88" t="s">
-        <v>135</v>
+        <v>302</v>
       </c>
       <c r="G88">
         <v>3</v>
       </c>
       <c r="H88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="I88">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>5</v>
       </c>
       <c r="B89">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="D89" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
       <c r="E89" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="F89" t="s">
-        <v>139</v>
+        <v>342</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H89">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I89">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>5</v>
       </c>
       <c r="B90">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C90" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E90" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F90" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G90">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="I90">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -3793,8 +4066,11 @@
       <c r="H91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -3802,16 +4078,16 @@
         <v>101</v>
       </c>
       <c r="C92" t="s">
+        <v>325</v>
+      </c>
+      <c r="D92" t="s">
         <v>326</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>327</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>328</v>
-      </c>
-      <c r="F92" t="s">
-        <v>329</v>
       </c>
       <c r="G92">
         <v>999</v>
@@ -3819,8 +4095,11 @@
       <c r="H92">
         <v>86</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -3828,16 +4107,16 @@
         <v>102</v>
       </c>
       <c r="C93" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D93" t="s">
+        <v>329</v>
+      </c>
+      <c r="E93" t="s">
         <v>330</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>331</v>
-      </c>
-      <c r="F93" t="s">
-        <v>332</v>
       </c>
       <c r="G93">
         <v>999</v>
@@ -3845,8 +4124,11 @@
       <c r="H93">
         <v>49</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -3857,13 +4139,13 @@
         <v>105</v>
       </c>
       <c r="D94" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E94" t="s">
         <v>67</v>
       </c>
       <c r="F94" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G94">
         <v>999</v>
@@ -3871,62 +4153,71 @@
       <c r="H94">
         <v>41</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
       <c r="B95">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C95" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D95" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E95" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F95" t="s">
-        <v>338</v>
+        <v>271</v>
       </c>
       <c r="G95">
         <v>999</v>
       </c>
       <c r="H95">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="I95">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
       <c r="B96">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C96" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D96" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E96" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F96" t="s">
-        <v>272</v>
+        <v>337</v>
       </c>
       <c r="G96">
         <v>999</v>
       </c>
       <c r="H96">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="I96">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H99">
-    <sortCondition descending="1" ref="A2:A99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I96">
+    <sortCondition ref="G2:G96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>